<commit_message>
Write operation on excel sheet for patient details
</commit_message>
<xml_diff>
--- a/datafiles/Book1.xlsx
+++ b/datafiles/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Username</t>
   </si>
@@ -48,22 +48,68 @@
     <t>Bhavana123</t>
   </si>
   <si>
-    <t>Divya</t>
-  </si>
-  <si>
-    <t>Divya123</t>
-  </si>
-  <si>
-    <t>Valli</t>
-  </si>
-  <si>
-    <t>Valli123</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Parent First Name</t>
+  </si>
+  <si>
+    <t>Parent Middle Name</t>
+  </si>
+  <si>
+    <t>Parent Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>middle name</t>
+  </si>
+  <si>
+    <t>Nannapaneni</t>
+  </si>
+  <si>
+    <t>Srinivas</t>
+  </si>
+  <si>
+    <t>Parent middle name</t>
+  </si>
+  <si>
+    <t>gnannap1@asu.edu</t>
+  </si>
+  <si>
+    <t>6026219441</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -389,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -437,22 +483,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -460,12 +490,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added all portal functionalities for user
</commit_message>
<xml_diff>
--- a/datafiles/Book1.xlsx
+++ b/datafiles/Book1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahit\Desktop\CSE project\PediaCare\datafiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DBA7CD-32E4-4542-93B5-1CB9A86513ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="57">
   <si>
     <t>Username</t>
   </si>
@@ -42,12 +48,6 @@
     <t>Geethika123</t>
   </si>
   <si>
-    <t>Bhavana</t>
-  </si>
-  <si>
-    <t>Bhavana123</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -103,17 +103,114 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Sahithi</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Boddupalli</t>
+  </si>
+  <si>
+    <t>Subbarao</t>
+  </si>
+  <si>
+    <t>brvsahithi@gmail.com</t>
+  </si>
+  <si>
+    <t>4123789908</t>
+  </si>
+  <si>
+    <t>1255 E University DR</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>1255 E University</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1225 E University dr</t>
+  </si>
+  <si>
+    <t>np</t>
+  </si>
+  <si>
+    <t>Sri</t>
+  </si>
+  <si>
+    <t>wsdyh@outlook.com</t>
+  </si>
+  <si>
+    <t>1258 W University Dr</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>john123</t>
+  </si>
+  <si>
+    <t>kenedy</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>1267 S Rural Rd</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>monica123</t>
+  </si>
+  <si>
+    <t>Geller</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>monica@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1157 N Broadway </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,17 +233,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -193,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,9 +333,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,6 +385,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,138 +578,422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>4123789908</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>7452397426</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5">
+        <v>8963254172</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>1236547891</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{BE1E925D-1645-48EA-A377-38B0413F9722}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{7F8B442A-E61C-433E-BE9A-21E195495EC1}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{CFAA42BF-C8BA-4FB6-AA64-E3F1D5F2A62C}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{F240C800-B3E8-4035-AD29-7B90B32CD33F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="B4" t="s">
         <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -574,12 +1002,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made final Backend changes
</commit_message>
<xml_diff>
--- a/datafiles/Book1.xlsx
+++ b/datafiles/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patient Login Creds" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Username</t>
   </si>
@@ -75,136 +75,122 @@
     <t>Speech Therapy</t>
   </si>
   <si>
-    <t>middle name</t>
+    <t>"4444"</t>
+  </si>
+  <si>
+    <t>"78789"</t>
+  </si>
+  <si>
+    <t>"8278732"</t>
+  </si>
+  <si>
+    <t>Previous Condition</t>
+  </si>
+  <si>
+    <t>Current Condition</t>
+  </si>
+  <si>
+    <t>Visit Sumary</t>
+  </si>
+  <si>
+    <t>Prescribed Medicines</t>
+  </si>
+  <si>
+    <t>Ear Pain</t>
+  </si>
+  <si>
+    <t>Skin Infection</t>
+  </si>
+  <si>
+    <t>Metoprolol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antipyrine </t>
+  </si>
+  <si>
+    <t>Prescibed medicines for skin infection has to visit after 4 weeks i.e 23-12-2021</t>
+  </si>
+  <si>
+    <t>Prescibed medicines for Ear has to visit after 3 weeks i.e 13-12-2021</t>
+  </si>
+  <si>
+    <t>skin Infection</t>
+  </si>
+  <si>
+    <t>ear Pain</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Doctor123</t>
+  </si>
+  <si>
+    <t>Doctor1</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Nurse123</t>
+  </si>
+  <si>
+    <t>Nurse1</t>
+  </si>
+  <si>
+    <t>Preferred Pharmacy</t>
+  </si>
+  <si>
+    <t>CVS Pharmacy</t>
+  </si>
+  <si>
+    <t>Safe way Pharmacy</t>
+  </si>
+  <si>
+    <t>Safeway Pharmacy</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>2021-1101</t>
   </si>
   <si>
     <t>Nannapaneni</t>
   </si>
   <si>
-    <t>Saisrinivas</t>
-  </si>
-  <si>
-    <t>Parent middle name</t>
-  </si>
-  <si>
-    <t>sss@gmail.com</t>
-  </si>
-  <si>
-    <t>78789788</t>
-  </si>
-  <si>
-    <t>nhdjhfjd@email.com</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>"4444"</t>
-  </si>
-  <si>
-    <t>"78789"</t>
-  </si>
-  <si>
-    <t>"8278732"</t>
-  </si>
-  <si>
-    <t>2021-11-04</t>
-  </si>
-  <si>
-    <t>Previous Condition</t>
-  </si>
-  <si>
-    <t>Current Condition</t>
-  </si>
-  <si>
-    <t>Visit Sumary</t>
-  </si>
-  <si>
-    <t>Prescribed Medicines</t>
-  </si>
-  <si>
-    <t>Ear Pain</t>
-  </si>
-  <si>
-    <t>Skin Infection</t>
-  </si>
-  <si>
-    <t>Metoprolol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antipyrine </t>
-  </si>
-  <si>
-    <t>Prescibed medicines for skin infection has to visit after 4 weeks i.e 23-12-2021</t>
-  </si>
-  <si>
-    <t>Prescibed medicines for Ear has to visit after 3 weeks i.e 13-12-2021</t>
-  </si>
-  <si>
-    <t>skin Infection</t>
-  </si>
-  <si>
-    <t>ear Pain</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>Doctor123</t>
-  </si>
-  <si>
-    <t>Doctor1</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Nurse</t>
-  </si>
-  <si>
-    <t>Nurse123</t>
-  </si>
-  <si>
-    <t>Nurse1</t>
-  </si>
-  <si>
-    <t>lljhjl</t>
-  </si>
-  <si>
-    <t>kljkl</t>
-  </si>
-  <si>
-    <t>kjl</t>
-  </si>
-  <si>
-    <t>klj</t>
-  </si>
-  <si>
-    <t>klnjkl</t>
-  </si>
-  <si>
-    <t>lkjnlkj</t>
-  </si>
-  <si>
-    <t>Preferred Pharmacy</t>
-  </si>
-  <si>
-    <t>CVS Pharmacy</t>
-  </si>
-  <si>
-    <t>Safe way Pharmacy</t>
-  </si>
-  <si>
-    <t>Safeway Pharmacy</t>
+    <t>Srinivas</t>
+  </si>
+  <si>
+    <t>gnannap1@asu.edu</t>
+  </si>
+  <si>
+    <t>333434</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>2021-11-11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -586,10 +572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -599,34 +585,34 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
         <v>6</v>
@@ -635,33 +621,10 @@
         <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="O1">
         <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -704,7 +667,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -721,7 +684,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -738,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -757,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -771,22 +734,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -797,22 +760,22 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -823,22 +786,22 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>102</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -849,22 +812,22 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>103</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -892,18 +855,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -923,18 +886,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>